<commit_message>
Enhance Excel export formatting: add background color and font color to various cell formats for improved readability.
</commit_message>
<xml_diff>
--- a/cash_flow_2025.xlsx
+++ b/cash_flow_2025.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="105">
   <si>
     <t>My cash flow for 2025 starting from 25/01/2025</t>
   </si>
@@ -67,12 +67,15 @@
     <t>Allowance from NYSC</t>
   </si>
   <si>
+    <t>________________     FEBRUARY    _________________</t>
+  </si>
+  <si>
+    <t>7/02/2025</t>
+  </si>
+  <si>
     <t>AGAM pays repayment on 900k from Miracle</t>
   </si>
   <si>
-    <t>________________     FEBRUARY    _________________</t>
-  </si>
-  <si>
     <t>10/02/2025</t>
   </si>
   <si>
@@ -196,6 +199,15 @@
     <t>30/06/2025</t>
   </si>
   <si>
+    <t>31/06/2025</t>
+  </si>
+  <si>
+    <t>Help AGAM to repay 700k Loan from Kenny</t>
+  </si>
+  <si>
+    <t>Give mom 600k to add to the 700k I help to pay Kenny, she should then use it to pay off Arowolo (800k), Honourable (400k) and Iyabo (100k) to make it the remaining 1.3m</t>
+  </si>
+  <si>
     <t>________________     JULY   _________________</t>
   </si>
   <si>
@@ -205,18 +217,6 @@
     <t>Repay part of OSCOFED 1.3m loan</t>
   </si>
   <si>
-    <t>08/07/2025</t>
-  </si>
-  <si>
-    <t>Pay remaining part of 800k loan from Honarable</t>
-  </si>
-  <si>
-    <t>Pay remaining part of 300k loan from Iyabo</t>
-  </si>
-  <si>
-    <t>Pay another part of 1.5m loan from Arowolo</t>
-  </si>
-  <si>
     <t>10/07/2025</t>
   </si>
   <si>
@@ -235,12 +235,6 @@
     <t>8/08/2025</t>
   </si>
   <si>
-    <t>08/08/2025</t>
-  </si>
-  <si>
-    <t>Pay remaining part of 1.5m loan from Arowolo</t>
-  </si>
-  <si>
     <t>10/08/2025</t>
   </si>
   <si>
@@ -253,12 +247,6 @@
     <t>31/08/2025</t>
   </si>
   <si>
-    <t>30/08/2025</t>
-  </si>
-  <si>
-    <t>Help AGAM to repay 800k Loan from Honarable</t>
-  </si>
-  <si>
     <t>________________     SEPTEMBER   _________________</t>
   </si>
   <si>
@@ -341,12 +329,6 @@
   </si>
   <si>
     <t>20/12/2025</t>
-  </si>
-  <si>
-    <t>31/21/2025</t>
-  </si>
-  <si>
-    <t>Help AGAM to repay 700k Loan from Kenny</t>
   </si>
 </sst>
 </file>
@@ -356,7 +338,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="₦ #,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,23 +363,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Times New Roman"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA0A0A4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -465,40 +447,40 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -795,7 +777,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F133"/>
+  <dimension ref="A1:F119"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -956,41 +938,41 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="6">
-        <v>1</v>
-      </c>
-      <c r="D10" s="7">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
+      <c r="D11" s="7">
         <v>90000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E11" s="7">
         <v>90000</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F11" s="11">
         <v>1178000</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
@@ -1007,10 +989,10 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C13" s="6">
         <v>1</v>
@@ -1027,10 +1009,10 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
@@ -1047,10 +1029,10 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" s="6">
         <v>5</v>
@@ -1067,10 +1049,10 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C16" s="6">
         <v>1</v>
@@ -1087,10 +1069,10 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -1107,10 +1089,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="6">
         <v>1</v>
@@ -1127,10 +1109,10 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
@@ -1147,10 +1129,10 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -1167,7 +1149,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>16</v>
@@ -1187,10 +1169,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
@@ -1207,10 +1189,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -1227,7 +1209,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1237,10 +1219,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
@@ -1257,10 +1239,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
@@ -1277,10 +1259,10 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
@@ -1297,10 +1279,10 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
@@ -1317,10 +1299,10 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
@@ -1337,10 +1319,10 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
@@ -1357,10 +1339,10 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
@@ -1377,10 +1359,10 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C32" s="6">
         <v>1</v>
@@ -1397,10 +1379,10 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
@@ -1417,10 +1399,10 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
@@ -1437,10 +1419,10 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C35" s="6">
         <v>1</v>
@@ -1457,10 +1439,10 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C36" s="6">
         <v>1</v>
@@ -1477,7 +1459,7 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>16</v>
@@ -1497,10 +1479,10 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
@@ -1517,7 +1499,7 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1527,10 +1509,10 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C40" s="6">
         <v>1</v>
@@ -1547,10 +1529,10 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C41" s="6">
         <v>1</v>
@@ -1567,10 +1549,10 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C42" s="6">
         <v>1</v>
@@ -1587,10 +1569,10 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
@@ -1607,10 +1589,10 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
@@ -1627,10 +1609,10 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C45" s="6">
         <v>1</v>
@@ -1647,10 +1629,10 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C46" s="6">
         <v>1</v>
@@ -1667,7 +1649,7 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B47" s="5" t="s">
         <v>16</v>
@@ -1687,10 +1669,10 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C48" s="6">
         <v>1</v>
@@ -1707,10 +1689,10 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C49" s="6">
         <v>5</v>
@@ -1727,7 +1709,7 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -1737,10 +1719,10 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C51" s="6">
         <v>1</v>
@@ -1757,10 +1739,10 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C52" s="6">
         <v>1</v>
@@ -1777,10 +1759,10 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C53" s="6">
         <v>1</v>
@@ -1797,10 +1779,10 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C54" s="6">
         <v>1</v>
@@ -1817,10 +1799,10 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C55" s="6">
         <v>1</v>
@@ -1837,10 +1819,10 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C56" s="6">
         <v>1</v>
@@ -1857,10 +1839,10 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
@@ -1877,7 +1859,7 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B58" s="5" t="s">
         <v>16</v>
@@ -1897,10 +1879,10 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
@@ -1917,7 +1899,7 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -1927,10 +1909,10 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C61" s="6">
         <v>1</v>
@@ -1947,10 +1929,10 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C62" s="6">
         <v>1</v>
@@ -1967,10 +1949,10 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
@@ -1987,10 +1969,10 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C64" s="6">
         <v>1</v>
@@ -2007,10 +1989,10 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
@@ -2027,10 +2009,10 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C66" s="6">
         <v>1</v>
@@ -2047,10 +2029,10 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C67" s="6">
         <v>1</v>
@@ -2067,7 +2049,7 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B68" s="5" t="s">
         <v>16</v>
@@ -2087,10 +2069,10 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C69" s="6">
         <v>1</v>
@@ -2106,153 +2088,153 @@
       </c>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
+      <c r="A70" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C70" s="6">
+        <v>1</v>
+      </c>
+      <c r="D70" s="10">
+        <v>-700000</v>
+      </c>
+      <c r="E70" s="10">
+        <v>-700000</v>
+      </c>
+      <c r="F70" s="11">
+        <v>1333000</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
         <v>61</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C71" s="6">
         <v>1</v>
       </c>
       <c r="D71" s="10">
-        <v>-120000</v>
+        <v>-600000</v>
       </c>
       <c r="E71" s="10">
-        <v>-120000</v>
-      </c>
-      <c r="F71" s="11">
-        <v>1913000</v>
+        <v>-600000</v>
+      </c>
+      <c r="F71" s="7">
+        <v>733000</v>
       </c>
     </row>
     <row r="72" spans="1:6">
-      <c r="A72" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B72" s="9" t="s">
+      <c r="A72" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="6">
-        <v>1</v>
-      </c>
-      <c r="D72" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="E72" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="F72" s="11">
-        <v>1513000</v>
-      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C73" s="6">
         <v>1</v>
       </c>
       <c r="D73" s="10">
-        <v>-100000</v>
+        <v>-120000</v>
       </c>
       <c r="E73" s="10">
-        <v>-100000</v>
-      </c>
-      <c r="F73" s="11">
-        <v>1413000</v>
+        <v>-120000</v>
+      </c>
+      <c r="F73" s="7">
+        <v>613000</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C74" s="6">
         <v>1</v>
       </c>
       <c r="D74" s="10">
-        <v>-400000</v>
+        <v>-50000</v>
       </c>
       <c r="E74" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="F74" s="11">
-        <v>1013000</v>
+        <v>-50000</v>
+      </c>
+      <c r="F74" s="7">
+        <v>563000</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C75" s="6">
         <v>1</v>
       </c>
-      <c r="D75" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E75" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="F75" s="7">
-        <v>963000</v>
+      <c r="D75" s="7">
+        <v>800000</v>
+      </c>
+      <c r="E75" s="7">
+        <v>800000</v>
+      </c>
+      <c r="F75" s="11">
+        <v>1363000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
       </c>
       <c r="D76" s="7">
-        <v>800000</v>
+        <v>168000</v>
       </c>
       <c r="E76" s="7">
-        <v>800000</v>
+        <v>168000</v>
       </c>
       <c r="F76" s="11">
-        <v>1763000</v>
+        <v>1531000</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B77" s="5" t="s">
-        <v>17</v>
+      <c r="B77" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C77" s="6">
         <v>1</v>
       </c>
-      <c r="D77" s="7">
-        <v>90000</v>
-      </c>
-      <c r="E77" s="7">
-        <v>90000</v>
+      <c r="D77" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E77" s="10">
+        <v>-168000</v>
       </c>
       <c r="F77" s="11">
-        <v>1853000</v>
+        <v>1363000</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2260,487 +2242,477 @@
         <v>70</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C78" s="6">
         <v>1</v>
       </c>
       <c r="D78" s="7">
-        <v>21000</v>
+        <v>33000</v>
       </c>
       <c r="E78" s="7">
-        <v>21000</v>
+        <v>33000</v>
       </c>
       <c r="F78" s="11">
-        <v>1874000</v>
+        <v>1396000</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>29</v>
+      <c r="B79" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C79" s="6">
         <v>1</v>
       </c>
-      <c r="D79" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E79" s="10">
-        <v>-21000</v>
+      <c r="D79" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E79" s="7">
+        <v>70000</v>
       </c>
       <c r="F79" s="11">
-        <v>1853000</v>
+        <v>1466000</v>
       </c>
     </row>
     <row r="80" spans="1:6">
-      <c r="A80" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C80" s="6">
-        <v>1</v>
-      </c>
-      <c r="D80" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E80" s="7">
-        <v>168000</v>
-      </c>
-      <c r="F80" s="11">
-        <v>2021000</v>
-      </c>
+      <c r="A80" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="C81" s="6">
         <v>1</v>
       </c>
       <c r="D81" s="10">
-        <v>-168000</v>
+        <v>-130000</v>
       </c>
       <c r="E81" s="10">
-        <v>-168000</v>
+        <v>-130000</v>
       </c>
       <c r="F81" s="11">
-        <v>1853000</v>
+        <v>1336000</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="5" t="s">
-        <v>16</v>
+        <v>73</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="C82" s="6">
         <v>1</v>
       </c>
-      <c r="D82" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E82" s="7">
-        <v>33000</v>
+      <c r="D82" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E82" s="10">
+        <v>-50000</v>
       </c>
       <c r="F82" s="11">
-        <v>1886000</v>
+        <v>1286000</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="4" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B83" s="5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C83" s="6">
         <v>1</v>
       </c>
       <c r="D83" s="7">
-        <v>70000</v>
+        <v>800000</v>
       </c>
       <c r="E83" s="7">
-        <v>70000</v>
+        <v>800000</v>
       </c>
       <c r="F83" s="11">
-        <v>1956000</v>
+        <v>2086000</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B84" s="3"/>
-      <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="A84" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C84" s="6">
+        <v>1</v>
+      </c>
+      <c r="D84" s="7">
+        <v>90000</v>
+      </c>
+      <c r="E84" s="7">
+        <v>90000</v>
+      </c>
+      <c r="F84" s="11">
+        <v>2176000</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>62</v>
+        <v>76</v>
+      </c>
+      <c r="B85" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C85" s="6">
         <v>1</v>
       </c>
-      <c r="D85" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E85" s="10">
-        <v>-130000</v>
+      <c r="D85" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E85" s="7">
+        <v>168000</v>
       </c>
       <c r="F85" s="11">
-        <v>1826000</v>
+        <v>2344000</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="C86" s="6">
         <v>1</v>
       </c>
       <c r="D86" s="10">
-        <v>-400000</v>
+        <v>-168000</v>
       </c>
       <c r="E86" s="10">
-        <v>-400000</v>
+        <v>-168000</v>
       </c>
       <c r="F86" s="11">
-        <v>1426000</v>
+        <v>2176000</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B87" s="9" t="s">
         <v>76</v>
       </c>
+      <c r="B87" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="C87" s="6">
         <v>1</v>
       </c>
-      <c r="D87" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E87" s="10">
-        <v>-50000</v>
+      <c r="D87" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E87" s="7">
+        <v>33000</v>
       </c>
       <c r="F87" s="11">
-        <v>1376000</v>
+        <v>2209000</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B88" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="6">
+        <v>1</v>
+      </c>
+      <c r="D88" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E88" s="7">
+        <v>70000</v>
+      </c>
+      <c r="F88" s="11">
+        <v>2279000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B88" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C88" s="6">
-        <v>1</v>
-      </c>
-      <c r="D88" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E88" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F88" s="11">
-        <v>2176000</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C89" s="6">
-        <v>1</v>
-      </c>
-      <c r="D89" s="7">
-        <v>90000</v>
-      </c>
-      <c r="E89" s="7">
-        <v>90000</v>
-      </c>
-      <c r="F89" s="11">
-        <v>2266000</v>
-      </c>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="3"/>
+      <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>28</v>
+      <c r="B90" s="9" t="s">
+        <v>66</v>
       </c>
       <c r="C90" s="6">
         <v>1</v>
       </c>
-      <c r="D90" s="7">
-        <v>21000</v>
-      </c>
-      <c r="E90" s="7">
-        <v>21000</v>
+      <c r="D90" s="10">
+        <v>-130000</v>
+      </c>
+      <c r="E90" s="10">
+        <v>-130000</v>
       </c>
       <c r="F90" s="11">
-        <v>2287000</v>
+        <v>2149000</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="C91" s="6">
         <v>1</v>
       </c>
       <c r="D91" s="10">
-        <v>-21000</v>
+        <v>-50000</v>
       </c>
       <c r="E91" s="10">
-        <v>-21000</v>
+        <v>-50000</v>
       </c>
       <c r="F91" s="11">
-        <v>2266000</v>
+        <v>2099000</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C92" s="6">
         <v>1</v>
       </c>
       <c r="D92" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="E92" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="F92" s="11">
-        <v>2434000</v>
+        <v>2899000</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>31</v>
+        <v>82</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C93" s="6">
         <v>1</v>
       </c>
-      <c r="D93" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E93" s="10">
-        <v>-168000</v>
+      <c r="D93" s="7">
+        <v>90000</v>
+      </c>
+      <c r="E93" s="7">
+        <v>90000</v>
       </c>
       <c r="F93" s="11">
-        <v>2266000</v>
+        <v>2989000</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C94" s="6">
         <v>1</v>
       </c>
       <c r="D94" s="7">
-        <v>33000</v>
+        <v>168000</v>
       </c>
       <c r="E94" s="7">
-        <v>33000</v>
+        <v>168000</v>
       </c>
       <c r="F94" s="11">
-        <v>2299000</v>
+        <v>3157000</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B95" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B95" s="9" t="s">
         <v>32</v>
       </c>
       <c r="C95" s="6">
         <v>1</v>
       </c>
-      <c r="D95" s="7">
-        <v>70000</v>
-      </c>
-      <c r="E95" s="7">
-        <v>70000</v>
+      <c r="D95" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E95" s="10">
+        <v>-168000</v>
       </c>
       <c r="F95" s="11">
-        <v>2369000</v>
+        <v>2989000</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B96" s="9" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="C96" s="6">
         <v>1</v>
       </c>
-      <c r="D96" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="E96" s="10">
-        <v>-400000</v>
+      <c r="D96" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E96" s="7">
+        <v>33000</v>
       </c>
       <c r="F96" s="11">
-        <v>1969000</v>
+        <v>3022000</v>
       </c>
     </row>
     <row r="97" spans="1:6">
-      <c r="A97" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
+      <c r="A97" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" s="6">
+        <v>1</v>
+      </c>
+      <c r="D97" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E97" s="7">
+        <v>70000</v>
+      </c>
+      <c r="F97" s="11">
+        <v>3092000</v>
+      </c>
     </row>
     <row r="98" spans="1:6">
-      <c r="A98" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="C98" s="6">
-        <v>1</v>
-      </c>
-      <c r="D98" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E98" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F98" s="11">
-        <v>1839000</v>
-      </c>
+      <c r="A98" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C99" s="6">
         <v>1</v>
       </c>
       <c r="D99" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="E99" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="F99" s="11">
-        <v>1789000</v>
+        <v>2962000</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B100" s="5" t="s">
-        <v>24</v>
+      <c r="B100" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C100" s="6">
         <v>1</v>
       </c>
-      <c r="D100" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E100" s="7">
-        <v>800000</v>
+      <c r="D100" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E100" s="10">
+        <v>-50000</v>
       </c>
       <c r="F100" s="11">
-        <v>2589000</v>
+        <v>2912000</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C101" s="6">
         <v>1</v>
       </c>
       <c r="D101" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E101" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F101" s="11">
-        <v>2679000</v>
+        <v>3712000</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C102" s="6">
         <v>1</v>
       </c>
-      <c r="D102" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E102" s="10">
-        <v>-21000</v>
+      <c r="D102" s="7">
+        <v>90000</v>
+      </c>
+      <c r="E102" s="7">
+        <v>90000</v>
       </c>
       <c r="F102" s="11">
-        <v>2658000</v>
+        <v>3802000</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C103" s="6">
         <v>1</v>
@@ -2752,15 +2724,15 @@
         <v>168000</v>
       </c>
       <c r="F103" s="11">
-        <v>2826000</v>
+        <v>3970000</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C104" s="6">
         <v>1</v>
@@ -2772,35 +2744,35 @@
         <v>-168000</v>
       </c>
       <c r="F104" s="11">
-        <v>2658000</v>
+        <v>3802000</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B105" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C105" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D105" s="7">
         <v>33000</v>
       </c>
       <c r="E105" s="7">
-        <v>33000</v>
+        <v>66000</v>
       </c>
       <c r="F105" s="11">
-        <v>2691000</v>
+        <v>3868000</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C106" s="6">
         <v>1</v>
@@ -2812,12 +2784,12 @@
         <v>70000</v>
       </c>
       <c r="F106" s="11">
-        <v>2761000</v>
+        <v>3938000</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2827,10 +2799,10 @@
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C108" s="6">
         <v>1</v>
@@ -2842,15 +2814,15 @@
         <v>-130000</v>
       </c>
       <c r="F108" s="11">
-        <v>2631000</v>
+        <v>3808000</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="4" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C109" s="6">
         <v>1</v>
@@ -2862,15 +2834,15 @@
         <v>-50000</v>
       </c>
       <c r="F109" s="11">
-        <v>2581000</v>
+        <v>3758000</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C110" s="6">
         <v>1</v>
@@ -2882,464 +2854,194 @@
         <v>800000</v>
       </c>
       <c r="F110" s="11">
-        <v>3381000</v>
+        <v>4558000</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C111" s="6">
         <v>1</v>
       </c>
       <c r="D111" s="7">
-        <v>90000</v>
+        <v>168000</v>
       </c>
       <c r="E111" s="7">
-        <v>90000</v>
+        <v>168000</v>
       </c>
       <c r="F111" s="11">
-        <v>3471000</v>
+        <v>4726000</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>28</v>
+        <v>94</v>
+      </c>
+      <c r="B112" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C112" s="6">
         <v>1</v>
       </c>
-      <c r="D112" s="7">
-        <v>21000</v>
-      </c>
-      <c r="E112" s="7">
-        <v>21000</v>
+      <c r="D112" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E112" s="10">
+        <v>-168000</v>
       </c>
       <c r="F112" s="11">
-        <v>3492000</v>
+        <v>4558000</v>
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B113" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C113" s="6">
-        <v>1</v>
-      </c>
-      <c r="D113" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E113" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="F113" s="11">
-        <v>3471000</v>
-      </c>
+      <c r="A113" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+      <c r="D113" s="3"/>
+      <c r="E113" s="3"/>
+      <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>30</v>
+        <v>96</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>97</v>
       </c>
       <c r="C114" s="6">
         <v>1</v>
       </c>
-      <c r="D114" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E114" s="7">
-        <v>168000</v>
+      <c r="D114" s="10">
+        <v>-260000</v>
+      </c>
+      <c r="E114" s="10">
+        <v>-260000</v>
       </c>
       <c r="F114" s="11">
-        <v>3639000</v>
+        <v>4298000</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="C115" s="6">
         <v>1</v>
       </c>
       <c r="D115" s="10">
-        <v>-168000</v>
+        <v>-50000</v>
       </c>
       <c r="E115" s="10">
-        <v>-168000</v>
+        <v>-50000</v>
       </c>
       <c r="F115" s="11">
-        <v>3471000</v>
+        <v>4248000</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B116" s="5" t="s">
-        <v>16</v>
+        <v>100</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="C116" s="6">
-        <v>2</v>
-      </c>
-      <c r="D116" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E116" s="7">
-        <v>66000</v>
+        <v>1</v>
+      </c>
+      <c r="D116" s="10">
+        <v>-300000</v>
+      </c>
+      <c r="E116" s="10">
+        <v>-300000</v>
       </c>
       <c r="F116" s="11">
-        <v>3537000</v>
+        <v>3948000</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B117" s="5" t="s">
-        <v>32</v>
+        <v>100</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>102</v>
       </c>
       <c r="C117" s="6">
         <v>1</v>
       </c>
-      <c r="D117" s="7">
-        <v>70000</v>
-      </c>
-      <c r="E117" s="7">
-        <v>70000</v>
+      <c r="D117" s="10">
+        <v>-100000</v>
+      </c>
+      <c r="E117" s="10">
+        <v>-100000</v>
       </c>
       <c r="F117" s="11">
-        <v>3607000</v>
+        <v>3848000</v>
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
+      <c r="A118" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C118" s="6">
+        <v>1</v>
+      </c>
+      <c r="D118" s="10">
+        <v>-100000</v>
+      </c>
+      <c r="E118" s="10">
+        <v>-100000</v>
+      </c>
+      <c r="F118" s="11">
+        <v>3748000</v>
+      </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B119" s="9" t="s">
-        <v>62</v>
+        <v>104</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="C119" s="6">
         <v>1</v>
       </c>
-      <c r="D119" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E119" s="10">
-        <v>-130000</v>
+      <c r="D119" s="7">
+        <v>800000</v>
+      </c>
+      <c r="E119" s="7">
+        <v>800000</v>
       </c>
       <c r="F119" s="11">
-        <v>3477000</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6">
-      <c r="A120" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B120" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C120" s="6">
-        <v>1</v>
-      </c>
-      <c r="D120" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E120" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="F120" s="11">
-        <v>3427000</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6">
-      <c r="A121" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C121" s="6">
-        <v>1</v>
-      </c>
-      <c r="D121" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E121" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F121" s="11">
-        <v>4227000</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6">
-      <c r="A122" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B122" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C122" s="6">
-        <v>1</v>
-      </c>
-      <c r="D122" s="7">
-        <v>21000</v>
-      </c>
-      <c r="E122" s="7">
-        <v>21000</v>
-      </c>
-      <c r="F122" s="11">
-        <v>4248000</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6">
-      <c r="A123" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B123" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C123" s="6">
-        <v>1</v>
-      </c>
-      <c r="D123" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E123" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="F123" s="11">
-        <v>4227000</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6">
-      <c r="A124" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B124" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C124" s="6">
-        <v>1</v>
-      </c>
-      <c r="D124" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E124" s="7">
-        <v>168000</v>
-      </c>
-      <c r="F124" s="11">
-        <v>4395000</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6">
-      <c r="A125" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B125" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C125" s="6">
-        <v>1</v>
-      </c>
-      <c r="D125" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E125" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="F125" s="11">
-        <v>4227000</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6">
-      <c r="A126" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-    </row>
-    <row r="127" spans="1:6">
-      <c r="A127" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B127" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="C127" s="6">
-        <v>1</v>
-      </c>
-      <c r="D127" s="10">
-        <v>-260000</v>
-      </c>
-      <c r="E127" s="10">
-        <v>-260000</v>
-      </c>
-      <c r="F127" s="11">
-        <v>3967000</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6">
-      <c r="A128" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C128" s="6">
-        <v>1</v>
-      </c>
-      <c r="D128" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E128" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="F128" s="11">
-        <v>3917000</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6">
-      <c r="A129" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B129" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="C129" s="6">
-        <v>1</v>
-      </c>
-      <c r="D129" s="10">
-        <v>-300000</v>
-      </c>
-      <c r="E129" s="10">
-        <v>-300000</v>
-      </c>
-      <c r="F129" s="11">
-        <v>3617000</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6">
-      <c r="A130" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B130" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C130" s="6">
-        <v>1</v>
-      </c>
-      <c r="D130" s="10">
-        <v>-100000</v>
-      </c>
-      <c r="E130" s="10">
-        <v>-100000</v>
-      </c>
-      <c r="F130" s="11">
-        <v>3517000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6">
-      <c r="A131" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="C131" s="6">
-        <v>1</v>
-      </c>
-      <c r="D131" s="10">
-        <v>-100000</v>
-      </c>
-      <c r="E131" s="10">
-        <v>-100000</v>
-      </c>
-      <c r="F131" s="11">
-        <v>3417000</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6">
-      <c r="A132" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B132" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C132" s="6">
-        <v>1</v>
-      </c>
-      <c r="D132" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E132" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F132" s="11">
-        <v>4217000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6">
-      <c r="A133" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B133" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="C133" s="6">
-        <v>1</v>
-      </c>
-      <c r="D133" s="10">
-        <v>-700000</v>
-      </c>
-      <c r="E133" s="10">
-        <v>-700000</v>
-      </c>
-      <c r="F133" s="11">
-        <v>3517000</v>
+        <v>4548000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A39:F39"/>
     <mergeCell ref="A50:F50"/>
     <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="A84:F84"/>
-    <mergeCell ref="A97:F97"/>
+    <mergeCell ref="A72:F72"/>
+    <mergeCell ref="A80:F80"/>
+    <mergeCell ref="A89:F89"/>
+    <mergeCell ref="A98:F98"/>
     <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A118:F118"/>
-    <mergeCell ref="A126:F126"/>
+    <mergeCell ref="A113:F113"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Update cash flow data: add new repayment entry and adjust existing repayment amount for accuracy. Enhance README with detailed repayment plan for the year.
</commit_message>
<xml_diff>
--- a/cash_flow_2025.xlsx
+++ b/cash_flow_2025.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="107">
   <si>
     <t>My cash flow for 2025 starting from 25/01/2025</t>
   </si>
@@ -59,6 +59,12 @@
   </si>
   <si>
     <t>Kenny repayed out of 250k loan given to her ✅</t>
+  </si>
+  <si>
+    <t>30/01/2025</t>
+  </si>
+  <si>
+    <t>Kenny completed repayment of 250k loan given to her ✅</t>
   </si>
   <si>
     <t>31/01/2025</t>
@@ -777,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -928,63 +934,63 @@
         <v>1</v>
       </c>
       <c r="D9" s="7">
+        <v>50000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>50000</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1105000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
         <v>33000</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="7">
         <v>33000</v>
       </c>
-      <c r="F9" s="11">
-        <v>1088000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="F10" s="11">
+        <v>1138000</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="6">
-        <v>1</v>
-      </c>
-      <c r="D11" s="7">
-        <v>90000</v>
-      </c>
-      <c r="E11" s="7">
-        <v>90000</v>
-      </c>
-      <c r="F11" s="11">
-        <v>1178000</v>
-      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="6">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E12" s="10">
-        <v>-50000</v>
+      <c r="D12" s="7">
+        <v>90000</v>
+      </c>
+      <c r="E12" s="7">
+        <v>90000</v>
       </c>
       <c r="F12" s="11">
-        <v>1128000</v>
+        <v>1228000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -998,1164 +1004,1164 @@
         <v>1</v>
       </c>
       <c r="D13" s="10">
-        <v>-130000</v>
+        <v>-50000</v>
       </c>
       <c r="E13" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F13" s="7">
-        <v>998000</v>
+        <v>-50000</v>
+      </c>
+      <c r="F13" s="11">
+        <v>1178000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C14" s="6">
         <v>1</v>
       </c>
-      <c r="D14" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E14" s="7">
-        <v>800000</v>
+      <c r="D14" s="10">
+        <v>-130000</v>
+      </c>
+      <c r="E14" s="10">
+        <v>-130000</v>
       </c>
       <c r="F14" s="11">
-        <v>1798000</v>
+        <v>1048000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="6">
-        <v>5</v>
-      </c>
-      <c r="D15" s="10">
-        <v>-300000</v>
-      </c>
-      <c r="E15" s="10">
-        <v>-1500000</v>
-      </c>
-      <c r="F15" s="7">
-        <v>298000</v>
+        <v>1</v>
+      </c>
+      <c r="D15" s="7">
+        <v>800000</v>
+      </c>
+      <c r="E15" s="7">
+        <v>800000</v>
+      </c>
+      <c r="F15" s="11">
+        <v>1848000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
+      <c r="B16" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="C16" s="6">
-        <v>1</v>
-      </c>
-      <c r="D16" s="7">
-        <v>90000</v>
-      </c>
-      <c r="E16" s="7">
-        <v>90000</v>
+        <v>5</v>
+      </c>
+      <c r="D16" s="10">
+        <v>-300000</v>
+      </c>
+      <c r="E16" s="10">
+        <v>-1500000</v>
       </c>
       <c r="F16" s="7">
-        <v>388000</v>
+        <v>348000</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
       </c>
       <c r="D17" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="E17" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="F17" s="7">
-        <v>409000</v>
+        <v>438000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="9" t="s">
         <v>30</v>
       </c>
+      <c r="B18" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C18" s="6">
         <v>1</v>
       </c>
-      <c r="D18" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E18" s="10">
-        <v>-21000</v>
+      <c r="D18" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E18" s="7">
+        <v>21000</v>
       </c>
       <c r="F18" s="7">
-        <v>388000</v>
+        <v>459000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C19" s="6">
         <v>1</v>
       </c>
-      <c r="D19" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E19" s="7">
-        <v>168000</v>
+      <c r="D19" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="E19" s="10">
+        <v>-21000</v>
       </c>
       <c r="F19" s="7">
-        <v>556000</v>
+        <v>438000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
       </c>
-      <c r="D20" s="10">
-        <v>-118000</v>
-      </c>
-      <c r="E20" s="10">
-        <v>-118000</v>
+      <c r="D20" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E20" s="7">
+        <v>168000</v>
       </c>
       <c r="F20" s="7">
-        <v>438000</v>
+        <v>606000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C21" s="6">
         <v>1</v>
       </c>
-      <c r="D21" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E21" s="7">
-        <v>33000</v>
+      <c r="D21" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E21" s="10">
+        <v>-168000</v>
       </c>
       <c r="F21" s="7">
-        <v>471000</v>
+        <v>438000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C22" s="6">
         <v>1</v>
       </c>
       <c r="D22" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="E22" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="F22" s="7">
-        <v>541000</v>
+        <v>471000</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E23" s="7">
+        <v>70000</v>
+      </c>
+      <c r="F23" s="7">
+        <v>541000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="D24" s="10">
         <v>-400000</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E24" s="10">
         <v>-400000</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F24" s="7">
         <v>141000</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-    </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="6">
-        <v>1</v>
-      </c>
-      <c r="D25" s="10">
-        <v>-40000</v>
-      </c>
-      <c r="E25" s="10">
-        <v>-40000</v>
-      </c>
-      <c r="F25" s="7">
-        <v>101000</v>
-      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
-      <c r="D26" s="7">
-        <v>1300000</v>
-      </c>
-      <c r="E26" s="7">
-        <v>1300000</v>
-      </c>
-      <c r="F26" s="11">
-        <v>1401000</v>
+      <c r="D26" s="10">
+        <v>-40000</v>
+      </c>
+      <c r="E26" s="10">
+        <v>-40000</v>
+      </c>
+      <c r="F26" s="7">
+        <v>101000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="9" t="s">
         <v>40</v>
       </c>
+      <c r="B27" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
-      <c r="D27" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="E27" s="10">
-        <v>-400000</v>
+      <c r="D27" s="7">
+        <v>1300000</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1300000</v>
       </c>
       <c r="F27" s="11">
-        <v>1001000</v>
+        <v>1401000</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
       </c>
       <c r="D28" s="10">
-        <v>-200000</v>
+        <v>-400000</v>
       </c>
       <c r="E28" s="10">
-        <v>-200000</v>
-      </c>
-      <c r="F28" s="7">
-        <v>801000</v>
+        <v>-400000</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1001000</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="10">
-        <v>-700000</v>
+        <v>-200000</v>
       </c>
       <c r="E29" s="10">
-        <v>-700000</v>
+        <v>-200000</v>
       </c>
       <c r="F29" s="7">
-        <v>101000</v>
+        <v>801000</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>25</v>
+        <v>40</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>44</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
       </c>
-      <c r="D30" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E30" s="7">
-        <v>800000</v>
+      <c r="D30" s="10">
+        <v>-700000</v>
+      </c>
+      <c r="E30" s="10">
+        <v>-700000</v>
       </c>
       <c r="F30" s="7">
-        <v>901000</v>
+        <v>101000</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="9" t="s">
         <v>45</v>
       </c>
+      <c r="B31" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="C31" s="6">
         <v>1</v>
       </c>
-      <c r="D31" s="10">
-        <v>-400000</v>
-      </c>
-      <c r="E31" s="10">
-        <v>-400000</v>
+      <c r="D31" s="7">
+        <v>800000</v>
+      </c>
+      <c r="E31" s="7">
+        <v>800000</v>
       </c>
       <c r="F31" s="7">
-        <v>501000</v>
+        <v>901000</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>19</v>
+      <c r="B32" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C32" s="6">
         <v>1</v>
       </c>
-      <c r="D32" s="7">
-        <v>90000</v>
-      </c>
-      <c r="E32" s="7">
-        <v>90000</v>
+      <c r="D32" s="10">
+        <v>-400000</v>
+      </c>
+      <c r="E32" s="10">
+        <v>-400000</v>
       </c>
       <c r="F32" s="7">
-        <v>591000</v>
+        <v>501000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C33" s="6">
         <v>1</v>
       </c>
       <c r="D33" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="E33" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="F33" s="7">
-        <v>612000</v>
+        <v>591000</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>30</v>
+        <v>48</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C34" s="6">
         <v>1</v>
       </c>
-      <c r="D34" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E34" s="10">
-        <v>-21000</v>
+      <c r="D34" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E34" s="7">
+        <v>21000</v>
       </c>
       <c r="F34" s="7">
-        <v>591000</v>
+        <v>612000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C35" s="6">
         <v>1</v>
       </c>
-      <c r="D35" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E35" s="7">
-        <v>168000</v>
+      <c r="D35" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="E35" s="10">
+        <v>-21000</v>
       </c>
       <c r="F35" s="7">
-        <v>759000</v>
+        <v>591000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>32</v>
+        <v>48</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C36" s="6">
         <v>1</v>
       </c>
-      <c r="D36" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E36" s="10">
-        <v>-168000</v>
+      <c r="D36" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E36" s="7">
+        <v>168000</v>
       </c>
       <c r="F36" s="7">
-        <v>591000</v>
+        <v>759000</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>16</v>
+        <v>48</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C37" s="6">
         <v>1</v>
       </c>
-      <c r="D37" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E37" s="7">
-        <v>33000</v>
+      <c r="D37" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E37" s="10">
+        <v>-168000</v>
       </c>
       <c r="F37" s="7">
-        <v>624000</v>
+        <v>591000</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
       <c r="D38" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E38" s="7">
+        <v>33000</v>
+      </c>
+      <c r="F38" s="7">
+        <v>624000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1</v>
+      </c>
+      <c r="D39" s="7">
         <v>70000</v>
       </c>
-      <c r="E38" s="7">
+      <c r="E39" s="7">
         <v>70000</v>
       </c>
-      <c r="F38" s="7">
+      <c r="F39" s="7">
         <v>694000</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="6">
-        <v>1</v>
-      </c>
-      <c r="D40" s="10">
-        <v>-40000</v>
-      </c>
-      <c r="E40" s="10">
-        <v>-40000</v>
-      </c>
-      <c r="F40" s="7">
-        <v>654000</v>
-      </c>
+      <c r="A40" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C41" s="6">
         <v>1</v>
       </c>
-      <c r="D41" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E41" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F41" s="11">
-        <v>1454000</v>
+      <c r="D41" s="10">
+        <v>-40000</v>
+      </c>
+      <c r="E41" s="10">
+        <v>-40000</v>
+      </c>
+      <c r="F41" s="7">
+        <v>654000</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C42" s="6">
         <v>1</v>
       </c>
       <c r="D42" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E42" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F42" s="11">
-        <v>1544000</v>
+        <v>1454000</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C43" s="6">
         <v>1</v>
       </c>
       <c r="D43" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="E43" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="F43" s="11">
-        <v>1565000</v>
+        <v>1544000</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>30</v>
+        <v>52</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C44" s="6">
         <v>1</v>
       </c>
-      <c r="D44" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E44" s="10">
-        <v>-21000</v>
+      <c r="D44" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E44" s="7">
+        <v>21000</v>
       </c>
       <c r="F44" s="11">
-        <v>1544000</v>
+        <v>1565000</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>31</v>
+        <v>52</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C45" s="6">
         <v>1</v>
       </c>
-      <c r="D45" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E45" s="7">
-        <v>168000</v>
+      <c r="D45" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="E45" s="10">
+        <v>-21000</v>
       </c>
       <c r="F45" s="11">
-        <v>1712000</v>
+        <v>1544000</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="9" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C46" s="6">
         <v>1</v>
       </c>
-      <c r="D46" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E46" s="10">
-        <v>-168000</v>
+      <c r="D46" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E46" s="7">
+        <v>168000</v>
       </c>
       <c r="F46" s="11">
-        <v>1544000</v>
+        <v>1712000</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>16</v>
+        <v>52</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C47" s="6">
         <v>1</v>
       </c>
-      <c r="D47" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E47" s="7">
-        <v>33000</v>
+      <c r="D47" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E47" s="10">
+        <v>-168000</v>
       </c>
       <c r="F47" s="11">
-        <v>1577000</v>
+        <v>1544000</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C48" s="6">
         <v>1</v>
       </c>
       <c r="D48" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="E48" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="F48" s="11">
-        <v>1647000</v>
+        <v>1577000</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>27</v>
+        <v>52</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C49" s="6">
+        <v>1</v>
+      </c>
+      <c r="D49" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E49" s="7">
+        <v>70000</v>
+      </c>
+      <c r="F49" s="11">
+        <v>1647000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" s="6">
         <v>5</v>
       </c>
-      <c r="D49" s="10">
+      <c r="D50" s="10">
         <v>-300000</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E50" s="10">
         <v>-1500000</v>
       </c>
-      <c r="F49" s="7">
+      <c r="F50" s="7">
         <v>147000</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
-      <c r="A50" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="9" t="s">
+      <c r="A51" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C51" s="6">
-        <v>1</v>
-      </c>
-      <c r="D51" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E51" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="F51" s="12">
-        <v>97000</v>
-      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>25</v>
+      <c r="B52" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C52" s="6">
         <v>1</v>
       </c>
-      <c r="D52" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E52" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F52" s="7">
-        <v>897000</v>
+      <c r="D52" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E52" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="F52" s="12">
+        <v>97000</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C53" s="6">
         <v>1</v>
       </c>
       <c r="D53" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E53" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F53" s="7">
-        <v>987000</v>
+        <v>897000</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C54" s="6">
         <v>1</v>
       </c>
       <c r="D54" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="E54" s="7">
-        <v>21000</v>
-      </c>
-      <c r="F54" s="11">
-        <v>1008000</v>
+        <v>90000</v>
+      </c>
+      <c r="F54" s="7">
+        <v>987000</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B55" s="9" t="s">
-        <v>30</v>
+        <v>57</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C55" s="6">
         <v>1</v>
       </c>
-      <c r="D55" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E55" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="F55" s="7">
-        <v>987000</v>
+      <c r="D55" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E55" s="7">
+        <v>21000</v>
+      </c>
+      <c r="F55" s="11">
+        <v>1008000</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>31</v>
+        <v>57</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C56" s="6">
         <v>1</v>
       </c>
-      <c r="D56" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E56" s="7">
-        <v>168000</v>
-      </c>
-      <c r="F56" s="11">
-        <v>1155000</v>
+      <c r="D56" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="E56" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="F56" s="7">
+        <v>987000</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="9" t="s">
-        <v>32</v>
+        <v>57</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C57" s="6">
         <v>1</v>
       </c>
-      <c r="D57" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E57" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="F57" s="7">
-        <v>987000</v>
+      <c r="D57" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E57" s="7">
+        <v>168000</v>
+      </c>
+      <c r="F57" s="11">
+        <v>1155000</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="5" t="s">
-        <v>16</v>
+        <v>57</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C58" s="6">
         <v>1</v>
       </c>
-      <c r="D58" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E58" s="7">
-        <v>33000</v>
-      </c>
-      <c r="F58" s="11">
-        <v>1020000</v>
+      <c r="D58" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E58" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="F58" s="7">
+        <v>987000</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C59" s="6">
         <v>1</v>
       </c>
       <c r="D59" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E59" s="7">
+        <v>33000</v>
+      </c>
+      <c r="F59" s="11">
+        <v>1020000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="6">
+        <v>1</v>
+      </c>
+      <c r="D60" s="7">
         <v>70000</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E60" s="7">
         <v>70000</v>
       </c>
-      <c r="F59" s="11">
+      <c r="F60" s="11">
         <v>1090000</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
-      <c r="A60" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-    </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="B61" s="9" t="s">
+      <c r="A61" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="6">
-        <v>1</v>
-      </c>
-      <c r="D61" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="E61" s="10">
-        <v>-50000</v>
-      </c>
-      <c r="F61" s="11">
-        <v>1040000</v>
-      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>25</v>
+      <c r="B62" s="9" t="s">
+        <v>60</v>
       </c>
       <c r="C62" s="6">
         <v>1</v>
       </c>
-      <c r="D62" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E62" s="7">
-        <v>800000</v>
+      <c r="D62" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E62" s="10">
+        <v>-50000</v>
       </c>
       <c r="F62" s="11">
-        <v>1840000</v>
+        <v>1040000</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C63" s="6">
         <v>1</v>
       </c>
       <c r="D63" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E63" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F63" s="11">
-        <v>1930000</v>
+        <v>1840000</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C64" s="6">
         <v>1</v>
       </c>
       <c r="D64" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="E64" s="7">
-        <v>21000</v>
+        <v>90000</v>
       </c>
       <c r="F64" s="11">
-        <v>1951000</v>
+        <v>1930000</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>30</v>
+        <v>62</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C65" s="6">
         <v>1</v>
       </c>
-      <c r="D65" s="10">
-        <v>-21000</v>
-      </c>
-      <c r="E65" s="10">
-        <v>-21000</v>
+      <c r="D65" s="7">
+        <v>21000</v>
+      </c>
+      <c r="E65" s="7">
+        <v>21000</v>
       </c>
       <c r="F65" s="11">
-        <v>1930000</v>
+        <v>1951000</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="5" t="s">
-        <v>31</v>
+        <v>62</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>32</v>
       </c>
       <c r="C66" s="6">
         <v>1</v>
       </c>
-      <c r="D66" s="7">
-        <v>168000</v>
-      </c>
-      <c r="E66" s="7">
-        <v>168000</v>
+      <c r="D66" s="10">
+        <v>-21000</v>
+      </c>
+      <c r="E66" s="10">
+        <v>-21000</v>
       </c>
       <c r="F66" s="11">
-        <v>2098000</v>
+        <v>1930000</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>32</v>
+        <v>62</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C67" s="6">
         <v>1</v>
       </c>
-      <c r="D67" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E67" s="10">
-        <v>-168000</v>
+      <c r="D67" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E67" s="7">
+        <v>168000</v>
       </c>
       <c r="F67" s="11">
-        <v>1930000</v>
+        <v>2098000</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>16</v>
+        <v>62</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C68" s="6">
         <v>1</v>
       </c>
-      <c r="D68" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E68" s="7">
-        <v>33000</v>
+      <c r="D68" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E68" s="10">
+        <v>-168000</v>
       </c>
       <c r="F68" s="11">
-        <v>1963000</v>
+        <v>1930000</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C69" s="6">
         <v>1</v>
       </c>
       <c r="D69" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="E69" s="7">
-        <v>70000</v>
+        <v>33000</v>
       </c>
       <c r="F69" s="11">
-        <v>2033000</v>
+        <v>1963000</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B70" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="B70" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="C70" s="6">
         <v>1</v>
       </c>
-      <c r="D70" s="10">
-        <v>-700000</v>
-      </c>
-      <c r="E70" s="10">
-        <v>-700000</v>
+      <c r="D70" s="7">
+        <v>70000</v>
+      </c>
+      <c r="E70" s="7">
+        <v>70000</v>
       </c>
       <c r="F70" s="11">
-        <v>1333000</v>
+        <v>2033000</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="6">
+        <v>1</v>
+      </c>
+      <c r="D71" s="10">
+        <v>-700000</v>
+      </c>
+      <c r="E71" s="10">
+        <v>-700000</v>
+      </c>
+      <c r="F71" s="11">
+        <v>1333000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C71" s="6">
-        <v>1</v>
-      </c>
-      <c r="D71" s="10">
+      <c r="B72" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C72" s="6">
+        <v>1</v>
+      </c>
+      <c r="D72" s="10">
         <v>-600000</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E72" s="10">
         <v>-600000</v>
       </c>
-      <c r="F71" s="7">
+      <c r="F72" s="7">
         <v>733000</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="3"/>
-      <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-    </row>
     <row r="73" spans="1:6">
-      <c r="A73" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="9" t="s">
+      <c r="A73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="6">
-        <v>1</v>
-      </c>
-      <c r="D73" s="10">
-        <v>-120000</v>
-      </c>
-      <c r="E73" s="10">
-        <v>-120000</v>
-      </c>
-      <c r="F73" s="7">
-        <v>613000</v>
-      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
@@ -2168,764 +2174,764 @@
         <v>1</v>
       </c>
       <c r="D74" s="10">
-        <v>-50000</v>
+        <v>-120000</v>
       </c>
       <c r="E74" s="10">
-        <v>-50000</v>
+        <v>-120000</v>
       </c>
       <c r="F74" s="7">
-        <v>563000</v>
+        <v>613000</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>25</v>
+      <c r="B75" s="9" t="s">
+        <v>70</v>
       </c>
       <c r="C75" s="6">
         <v>1</v>
       </c>
-      <c r="D75" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E75" s="7">
-        <v>800000</v>
-      </c>
-      <c r="F75" s="11">
-        <v>1363000</v>
+      <c r="D75" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E75" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="F75" s="7">
+        <v>563000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="4" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B76" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C76" s="6">
         <v>1</v>
       </c>
       <c r="D76" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="E76" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="F76" s="11">
-        <v>1531000</v>
+        <v>1363000</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>32</v>
+        <v>72</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C77" s="6">
         <v>1</v>
       </c>
-      <c r="D77" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E77" s="10">
-        <v>-168000</v>
+      <c r="D77" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E77" s="7">
+        <v>168000</v>
       </c>
       <c r="F77" s="11">
-        <v>1363000</v>
+        <v>1531000</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>16</v>
+        <v>72</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C78" s="6">
         <v>1</v>
       </c>
-      <c r="D78" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E78" s="7">
-        <v>33000</v>
+      <c r="D78" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E78" s="10">
+        <v>-168000</v>
       </c>
       <c r="F78" s="11">
-        <v>1396000</v>
+        <v>1363000</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C79" s="6">
         <v>1</v>
       </c>
       <c r="D79" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E79" s="7">
+        <v>33000</v>
+      </c>
+      <c r="F79" s="11">
+        <v>1396000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B80" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C80" s="6">
+        <v>1</v>
+      </c>
+      <c r="D80" s="7">
         <v>70000</v>
       </c>
-      <c r="E79" s="7">
+      <c r="E80" s="7">
         <v>70000</v>
       </c>
-      <c r="F79" s="11">
+      <c r="F80" s="11">
         <v>1466000</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B80" s="3"/>
-      <c r="C80" s="3"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
-    </row>
     <row r="81" spans="1:6">
-      <c r="A81" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C81" s="6">
-        <v>1</v>
-      </c>
-      <c r="D81" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E81" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F81" s="11">
-        <v>1336000</v>
-      </c>
+      <c r="A81" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" s="3"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C82" s="6">
         <v>1</v>
       </c>
       <c r="D82" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="E82" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="F82" s="11">
-        <v>1286000</v>
+        <v>1336000</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="5" t="s">
-        <v>25</v>
+      <c r="B83" s="9" t="s">
+        <v>76</v>
       </c>
       <c r="C83" s="6">
         <v>1</v>
       </c>
-      <c r="D83" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E83" s="7">
-        <v>800000</v>
+      <c r="D83" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E83" s="10">
+        <v>-50000</v>
       </c>
       <c r="F83" s="11">
-        <v>2086000</v>
+        <v>1286000</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C84" s="6">
         <v>1</v>
       </c>
       <c r="D84" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E84" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F84" s="11">
-        <v>2176000</v>
+        <v>2086000</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C85" s="6">
         <v>1</v>
       </c>
       <c r="D85" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="E85" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="F85" s="11">
-        <v>2344000</v>
+        <v>2176000</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B86" s="9" t="s">
-        <v>32</v>
+        <v>78</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C86" s="6">
         <v>1</v>
       </c>
-      <c r="D86" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E86" s="10">
-        <v>-168000</v>
+      <c r="D86" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E86" s="7">
+        <v>168000</v>
       </c>
       <c r="F86" s="11">
-        <v>2176000</v>
+        <v>2344000</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B87" s="5" t="s">
-        <v>16</v>
+        <v>78</v>
+      </c>
+      <c r="B87" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C87" s="6">
         <v>1</v>
       </c>
-      <c r="D87" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E87" s="7">
-        <v>33000</v>
+      <c r="D87" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E87" s="10">
+        <v>-168000</v>
       </c>
       <c r="F87" s="11">
-        <v>2209000</v>
+        <v>2176000</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C88" s="6">
         <v>1</v>
       </c>
       <c r="D88" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E88" s="7">
+        <v>33000</v>
+      </c>
+      <c r="F88" s="11">
+        <v>2209000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B89" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C89" s="6">
+        <v>1</v>
+      </c>
+      <c r="D89" s="7">
         <v>70000</v>
       </c>
-      <c r="E88" s="7">
+      <c r="E89" s="7">
         <v>70000</v>
       </c>
-      <c r="F88" s="11">
+      <c r="F89" s="11">
         <v>2279000</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="B89" s="3"/>
-      <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
-    </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C90" s="6">
-        <v>1</v>
-      </c>
-      <c r="D90" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E90" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F90" s="11">
-        <v>2149000</v>
-      </c>
+      <c r="A90" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B91" s="9" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C91" s="6">
         <v>1</v>
       </c>
       <c r="D91" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="E91" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="F91" s="11">
-        <v>2099000</v>
+        <v>2149000</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B92" s="5" t="s">
-        <v>25</v>
+      <c r="B92" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="C92" s="6">
         <v>1</v>
       </c>
-      <c r="D92" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E92" s="7">
-        <v>800000</v>
+      <c r="D92" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E92" s="10">
+        <v>-50000</v>
       </c>
       <c r="F92" s="11">
-        <v>2899000</v>
+        <v>2099000</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C93" s="6">
         <v>1</v>
       </c>
       <c r="D93" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E93" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F93" s="11">
-        <v>2989000</v>
+        <v>2899000</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C94" s="6">
         <v>1</v>
       </c>
       <c r="D94" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="E94" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="F94" s="11">
-        <v>3157000</v>
+        <v>2989000</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B95" s="9" t="s">
-        <v>32</v>
+        <v>84</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C95" s="6">
         <v>1</v>
       </c>
-      <c r="D95" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E95" s="10">
-        <v>-168000</v>
+      <c r="D95" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E95" s="7">
+        <v>168000</v>
       </c>
       <c r="F95" s="11">
-        <v>2989000</v>
+        <v>3157000</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>16</v>
+        <v>84</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C96" s="6">
         <v>1</v>
       </c>
-      <c r="D96" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E96" s="7">
-        <v>33000</v>
+      <c r="D96" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E96" s="10">
+        <v>-168000</v>
       </c>
       <c r="F96" s="11">
-        <v>3022000</v>
+        <v>2989000</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C97" s="6">
         <v>1</v>
       </c>
       <c r="D97" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E97" s="7">
+        <v>33000</v>
+      </c>
+      <c r="F97" s="11">
+        <v>3022000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C98" s="6">
+        <v>1</v>
+      </c>
+      <c r="D98" s="7">
         <v>70000</v>
       </c>
-      <c r="E97" s="7">
+      <c r="E98" s="7">
         <v>70000</v>
       </c>
-      <c r="F97" s="11">
+      <c r="F98" s="11">
         <v>3092000</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-    </row>
     <row r="99" spans="1:6">
-      <c r="A99" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C99" s="6">
-        <v>1</v>
-      </c>
-      <c r="D99" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E99" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F99" s="11">
-        <v>2962000</v>
-      </c>
+      <c r="A99" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3"/>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C100" s="6">
         <v>1</v>
       </c>
       <c r="D100" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="E100" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="F100" s="11">
-        <v>2912000</v>
+        <v>2962000</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B101" s="5" t="s">
-        <v>25</v>
+      <c r="B101" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="C101" s="6">
         <v>1</v>
       </c>
-      <c r="D101" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E101" s="7">
-        <v>800000</v>
+      <c r="D101" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E101" s="10">
+        <v>-50000</v>
       </c>
       <c r="F101" s="11">
-        <v>3712000</v>
+        <v>2912000</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="C102" s="6">
         <v>1</v>
       </c>
       <c r="D102" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="E102" s="7">
-        <v>90000</v>
+        <v>800000</v>
       </c>
       <c r="F102" s="11">
-        <v>3802000</v>
+        <v>3712000</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C103" s="6">
         <v>1</v>
       </c>
       <c r="D103" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="E103" s="7">
-        <v>168000</v>
+        <v>90000</v>
       </c>
       <c r="F103" s="11">
-        <v>3970000</v>
+        <v>3802000</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>32</v>
+        <v>90</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C104" s="6">
         <v>1</v>
       </c>
-      <c r="D104" s="10">
-        <v>-168000</v>
-      </c>
-      <c r="E104" s="10">
-        <v>-168000</v>
+      <c r="D104" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E104" s="7">
+        <v>168000</v>
       </c>
       <c r="F104" s="11">
-        <v>3802000</v>
+        <v>3970000</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B105" s="5" t="s">
-        <v>16</v>
+        <v>90</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="C105" s="6">
-        <v>2</v>
-      </c>
-      <c r="D105" s="7">
-        <v>33000</v>
-      </c>
-      <c r="E105" s="7">
-        <v>66000</v>
+        <v>1</v>
+      </c>
+      <c r="D105" s="10">
+        <v>-168000</v>
+      </c>
+      <c r="E105" s="10">
+        <v>-168000</v>
       </c>
       <c r="F105" s="11">
-        <v>3868000</v>
+        <v>3802000</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="4" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="C106" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D106" s="7">
+        <v>33000</v>
+      </c>
+      <c r="E106" s="7">
+        <v>66000</v>
+      </c>
+      <c r="F106" s="11">
+        <v>3868000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C107" s="6">
+        <v>1</v>
+      </c>
+      <c r="D107" s="7">
         <v>70000</v>
       </c>
-      <c r="E106" s="7">
+      <c r="E107" s="7">
         <v>70000</v>
       </c>
-      <c r="F106" s="11">
+      <c r="F107" s="11">
         <v>3938000</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
-      <c r="A107" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B107" s="3"/>
-      <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-    </row>
     <row r="108" spans="1:6">
-      <c r="A108" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B108" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C108" s="6">
-        <v>1</v>
-      </c>
-      <c r="D108" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="E108" s="10">
-        <v>-130000</v>
-      </c>
-      <c r="F108" s="11">
-        <v>3808000</v>
-      </c>
+      <c r="A108" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C109" s="6">
         <v>1</v>
       </c>
       <c r="D109" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="E109" s="10">
-        <v>-50000</v>
+        <v>-130000</v>
       </c>
       <c r="F109" s="11">
-        <v>3758000</v>
+        <v>3808000</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B110" s="5" t="s">
-        <v>25</v>
+      <c r="B110" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="C110" s="6">
         <v>1</v>
       </c>
-      <c r="D110" s="7">
-        <v>800000</v>
-      </c>
-      <c r="E110" s="7">
-        <v>800000</v>
+      <c r="D110" s="10">
+        <v>-50000</v>
+      </c>
+      <c r="E110" s="10">
+        <v>-50000</v>
       </c>
       <c r="F110" s="11">
-        <v>4558000</v>
+        <v>3758000</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C111" s="6">
         <v>1</v>
       </c>
       <c r="D111" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="E111" s="7">
-        <v>168000</v>
+        <v>800000</v>
       </c>
       <c r="F111" s="11">
-        <v>4726000</v>
+        <v>4558000</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B112" s="9" t="s">
-        <v>32</v>
+        <v>96</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C112" s="6">
         <v>1</v>
       </c>
-      <c r="D112" s="10">
+      <c r="D112" s="7">
+        <v>168000</v>
+      </c>
+      <c r="E112" s="7">
+        <v>168000</v>
+      </c>
+      <c r="F112" s="11">
+        <v>4726000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C113" s="6">
+        <v>1</v>
+      </c>
+      <c r="D113" s="10">
         <v>-168000</v>
       </c>
-      <c r="E112" s="10">
+      <c r="E113" s="10">
         <v>-168000</v>
       </c>
-      <c r="F112" s="11">
+      <c r="F113" s="11">
         <v>4558000</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
-      <c r="A113" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B113" s="3"/>
-      <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3"/>
-    </row>
     <row r="114" spans="1:6">
-      <c r="A114" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B114" s="9" t="s">
+      <c r="A114" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C114" s="6">
-        <v>1</v>
-      </c>
-      <c r="D114" s="10">
-        <v>-260000</v>
-      </c>
-      <c r="E114" s="10">
-        <v>-260000</v>
-      </c>
-      <c r="F114" s="11">
-        <v>4298000</v>
-      </c>
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
+      <c r="E114" s="3"/>
+      <c r="F114" s="3"/>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="4" t="s">
@@ -2938,13 +2944,13 @@
         <v>1</v>
       </c>
       <c r="D115" s="10">
-        <v>-50000</v>
+        <v>-260000</v>
       </c>
       <c r="E115" s="10">
-        <v>-50000</v>
+        <v>-260000</v>
       </c>
       <c r="F115" s="11">
-        <v>4248000</v>
+        <v>4298000</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2958,41 +2964,41 @@
         <v>1</v>
       </c>
       <c r="D116" s="10">
-        <v>-300000</v>
+        <v>-50000</v>
       </c>
       <c r="E116" s="10">
-        <v>-300000</v>
+        <v>-50000</v>
       </c>
       <c r="F116" s="11">
-        <v>3948000</v>
+        <v>4248000</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C117" s="6">
         <v>1</v>
       </c>
       <c r="D117" s="10">
-        <v>-100000</v>
+        <v>-300000</v>
       </c>
       <c r="E117" s="10">
-        <v>-100000</v>
+        <v>-300000</v>
       </c>
       <c r="F117" s="11">
-        <v>3848000</v>
+        <v>3948000</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C118" s="6">
         <v>1</v>
@@ -3004,26 +3010,46 @@
         <v>-100000</v>
       </c>
       <c r="F118" s="11">
-        <v>3748000</v>
+        <v>3848000</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B119" s="5" t="s">
-        <v>25</v>
+        <v>102</v>
+      </c>
+      <c r="B119" s="9" t="s">
+        <v>105</v>
       </c>
       <c r="C119" s="6">
         <v>1</v>
       </c>
-      <c r="D119" s="7">
+      <c r="D119" s="10">
+        <v>-100000</v>
+      </c>
+      <c r="E119" s="10">
+        <v>-100000</v>
+      </c>
+      <c r="F119" s="11">
+        <v>3748000</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B120" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C120" s="6">
+        <v>1</v>
+      </c>
+      <c r="D120" s="7">
         <v>800000</v>
       </c>
-      <c r="E119" s="7">
+      <c r="E120" s="7">
         <v>800000</v>
       </c>
-      <c r="F119" s="11">
+      <c r="F120" s="11">
         <v>4548000</v>
       </c>
     </row>
@@ -3031,17 +3057,17 @@
   <mergeCells count="13">
     <mergeCell ref="A1:F2"/>
     <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A39:F39"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A60:F60"/>
-    <mergeCell ref="A72:F72"/>
-    <mergeCell ref="A80:F80"/>
-    <mergeCell ref="A89:F89"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A107:F107"/>
-    <mergeCell ref="A113:F113"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A61:F61"/>
+    <mergeCell ref="A73:F73"/>
+    <mergeCell ref="A81:F81"/>
+    <mergeCell ref="A90:F90"/>
+    <mergeCell ref="A99:F99"/>
+    <mergeCell ref="A108:F108"/>
+    <mergeCell ref="A114:F114"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>